<commit_message>
Commiting code and test data for specific case.
</commit_message>
<xml_diff>
--- a/resources/test_data/test_data.xlsx
+++ b/resources/test_data/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New_automation_\web-automation-framework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E94A6CA-B3CD-4C05-A0DD-4CDE8BC1EAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2131961D-7E8F-40BC-AFD1-4194DC7B9329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>disposeDate</t>
   </si>
@@ -85,13 +85,34 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>Valid Login Test 1</t>
+  </si>
+  <si>
+    <t>Valid Site Visit Test 2</t>
+  </si>
+  <si>
+    <t>ruleName</t>
+  </si>
+  <si>
+    <t>Pre DPD 1- 29 and OS AMT =&lt;3000000</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>2050088104</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,8 +140,28 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1D1A20"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,8 +174,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -153,11 +200,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -177,14 +237,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
     <dxf>
       <font>
         <b val="0"/>
@@ -221,6 +286,44 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -349,19 +452,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DC87E5BE-26EC-4DBC-8565-103061C7F3D4}" name="Table2" displayName="Table2" ref="A1:J4" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J4" xr:uid="{DC87E5BE-26EC-4DBC-8565-103061C7F3D4}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{F63B5B5B-75EF-415D-9D47-65053D6DF43A}" name="username" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00DFF19F-9E5D-44BD-B746-C5D10556D9C8}" name="password" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{967B1CEC-1373-4B37-B605-9DD555121E42}" name="disposeDate" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{16007208-EDF9-4E5D-AAA6-7F837DDD8C78}" name="actionDate" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{EBB0D839-0B51-4805-BD0B-AAB83E639E7A}" name="actionRemark" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{07BF2CBA-E818-4808-9F87-9C6E9B8E27EB}" name="disposition" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{2E161694-E056-49B2-B02C-18609B166288}" name="communicationMode" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{833F8941-B4C0-4E9B-89CA-6ACBE1BBC919}" name="dispositionBy" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{6AB217CA-8575-47C6-8323-49DBB8179C87}" name="remark" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{B427C861-36D2-4A49-8916-781C22F94FF4}" name="action" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DC87E5BE-26EC-4DBC-8565-103061C7F3D4}" name="Table2" displayName="Table2" ref="B1:M4" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="B1:M4" xr:uid="{DC87E5BE-26EC-4DBC-8565-103061C7F3D4}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{F63B5B5B-75EF-415D-9D47-65053D6DF43A}" name="username" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00DFF19F-9E5D-44BD-B746-C5D10556D9C8}" name="password" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{967B1CEC-1373-4B37-B605-9DD555121E42}" name="disposeDate" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{16007208-EDF9-4E5D-AAA6-7F837DDD8C78}" name="actionDate" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{EBB0D839-0B51-4805-BD0B-AAB83E639E7A}" name="actionRemark" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{07BF2CBA-E818-4808-9F87-9C6E9B8E27EB}" name="disposition" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{2E161694-E056-49B2-B02C-18609B166288}" name="communicationMode" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{833F8941-B4C0-4E9B-89CA-6ACBE1BBC919}" name="dispositionBy" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{6AB217CA-8575-47C6-8323-49DBB8179C87}" name="remark" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{B427C861-36D2-4A49-8916-781C22F94FF4}" name="action" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{BC30846C-2EA9-4DD7-B7FD-8EFA2281FD70}" name="ruleName" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{7521EBC7-8105-4B20-B089-0355970E2900}" name="CR" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -630,133 +735,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="30">
+      <c r="A1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="L1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="30">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:13" ht="45">
+      <c r="A2" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="3">
-        <v>45547.67291666667</v>
       </c>
       <c r="D2" s="3">
         <v>45547.67291666667</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3">
+        <v>45547.67291666667</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="30">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+    <row r="3" spans="1:13" ht="45">
+      <c r="A3" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C3">
-        <v>45547.631249999999</v>
       </c>
       <c r="D3" s="3">
         <v>45547.631249999999</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3">
+        <v>45547.631249999999</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="L3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="2"/>
+    <row r="4" spans="1:13">
       <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
-    <row r="8" spans="1:10">
-      <c r="E8" s="5"/>
+    <row r="8" spans="1:13">
+      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>